<commit_message>
Activities & Companies Changes After Db refresh - 30 Oct 2023
</commit_message>
<xml_diff>
--- a/TestData/T2041_Companies_FSCoverageTeam_VerifyRequiredFieldsHelpText.xlsx
+++ b/TestData/T2041_Companies_FSCoverageTeam_VerifyRequiredFieldsHelpText.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F2A0B1-D1C4-472D-A27C-387FA8A2CB12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B493DA59-77EB-4899-AD2A-15F0D1985B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9768" windowHeight="2952" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -120,13 +120,13 @@
     <t>A</t>
   </si>
   <si>
-    <t>Credit Fund</t>
-  </si>
-  <si>
-    <t>Sponsor Officer</t>
-  </si>
-  <si>
     <t>Jacklyn Robinson</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Education</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,13 +629,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>27</v>

</xml_diff>